<commit_message>
Lista de links atualizada com comandos Git
</commit_message>
<xml_diff>
--- a/Dev Links.xlsx
+++ b/Dev Links.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Dev list</t>
   </si>
@@ -84,6 +84,24 @@
   </si>
   <si>
     <t>http://daviwp.com/10-scripts-jquery-para-wordpress/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bancos de imagens </t>
+  </si>
+  <si>
+    <t>103 bancos de imagens gratúitos</t>
+  </si>
+  <si>
+    <t>http://marketingdeconteudo.com/melhores-bancos-de-imagens-gratuitos/</t>
+  </si>
+  <si>
+    <t>Comandos GIT</t>
+  </si>
+  <si>
+    <t>Lista de comandos GIT</t>
+  </si>
+  <si>
+    <t>https://gist.github.com/leocomelli/2545add34e4fec21ec16</t>
   </si>
 </sst>
 </file>
@@ -474,34 +492,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="30" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="53.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="69.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>3</v>
       </c>
     </row>
@@ -566,6 +584,78 @@
       <c r="C8" s="2" t="s">
         <v>19</v>
       </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="2"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="2"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="2"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="2"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="2"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="2"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="2"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="2"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="2"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -578,8 +668,9 @@
     <hyperlink ref="C6" r:id="rId4"/>
     <hyperlink ref="C7" r:id="rId5"/>
     <hyperlink ref="C8" r:id="rId6"/>
+    <hyperlink ref="C9" r:id="rId7"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId7"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId8"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Banco de imagens Pedro
</commit_message>
<xml_diff>
--- a/Dev Links.xlsx
+++ b/Dev Links.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>Dev list</t>
   </si>
@@ -102,6 +102,15 @@
   </si>
   <si>
     <t>https://gist.github.com/leocomelli/2545add34e4fec21ec16</t>
+  </si>
+  <si>
+    <t>Banco de Imagens</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Banco de Imagens Pedro </t>
+  </si>
+  <si>
+    <t>https://www.pexels.com/</t>
   </si>
 </sst>
 </file>
@@ -495,7 +504,7 @@
   <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -608,9 +617,15 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="2"/>
+      <c r="A11" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>

</xml_diff>